<commit_message>
added email adress in template
to test PR workflow
</commit_message>
<xml_diff>
--- a/templates/community/CMML/20240619_125512_phototrophic_cell_culture.xlsx
+++ b/templates/community/CMML/20240619_125512_phototrophic_cell_culture.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D48C8F-C316-407C-9804-714AFB92C382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1640" yWindow="2060" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="New Table" state="visible" r:id="rId5"/>
+    <sheet name="isa_template" sheetId="1" r:id="rId1"/>
+    <sheet name="New Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -276,19 +280,30 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>philipp.westhoff@hhu.de</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,13 +323,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AX2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:AX2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:AX2">
+  <autoFilter ref="A1:AX2" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -385,56 +403,56 @@
     <filterColumn colId="49" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="50">
-    <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Parameter [sample submission date]" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF ()" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number ()" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Characteristic [organism]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Term Source REF (OBI:0100026)" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Accession Number (OBI:0100026)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Characteristic [genotype]" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Term Source REF (EFO:0000513)" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Term Accession Number (EFO:0000513)" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Characteristic [biological replicate]" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Term Source REF (DPBO:0000042)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Term Accession Number (DPBO:0000042)" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Factor [condition]" totalsRowFunction="none"/>
-    <tableColumn id="15" name="Term Source REF () " totalsRowFunction="none"/>
-    <tableColumn id="16" name="Term Accession Number () " totalsRowFunction="none"/>
-    <tableColumn id="17" name="Factor [condition.2]" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Term Source REF ()  " totalsRowFunction="none"/>
-    <tableColumn id="19" name="Term Accession Number ()  " totalsRowFunction="none"/>
-    <tableColumn id="20" name="Factor [condition.3]" totalsRowFunction="none"/>
-    <tableColumn id="21" name="Term Source REF ()   " totalsRowFunction="none"/>
-    <tableColumn id="22" name="Term Accession Number ()   " totalsRowFunction="none"/>
-    <tableColumn id="23" name="Characteristic [Light Cycle]" totalsRowFunction="none"/>
-    <tableColumn id="24" name="Term Source REF (NCIT:C90419)" totalsRowFunction="none"/>
-    <tableColumn id="25" name="Term Accession Number (NCIT:C90419)" totalsRowFunction="none"/>
-    <tableColumn id="26" name="Characteristic [Light intensity]" totalsRowFunction="none"/>
-    <tableColumn id="27" name="Term Source REF ()    " totalsRowFunction="none"/>
-    <tableColumn id="28" name="Term Accession Number ()    " totalsRowFunction="none"/>
-    <tableColumn id="29" name="Characteristic [shaker rpm]" totalsRowFunction="none"/>
-    <tableColumn id="30" name="Term Source REF ()     " totalsRowFunction="none"/>
-    <tableColumn id="31" name="Term Accession Number ()     " totalsRowFunction="none"/>
-    <tableColumn id="32" name="Characteristic [cultivation device]" totalsRowFunction="none"/>
-    <tableColumn id="33" name="Term Source REF ()      " totalsRowFunction="none"/>
-    <tableColumn id="34" name="Term Accession Number ()      " totalsRowFunction="none"/>
-    <tableColumn id="35" name="Characteristic [cell number]" totalsRowFunction="none"/>
-    <tableColumn id="36" name="Term Source REF ()       " totalsRowFunction="none"/>
-    <tableColumn id="37" name="Term Accession Number ()       " totalsRowFunction="none"/>
-    <tableColumn id="38" name="Characteristic [OD units]" totalsRowFunction="none"/>
-    <tableColumn id="39" name="Term Source REF ()        " totalsRowFunction="none"/>
-    <tableColumn id="40" name="Term Accession Number ()        " totalsRowFunction="none"/>
-    <tableColumn id="41" name="Characteristic [sampling protocol]" totalsRowFunction="none"/>
-    <tableColumn id="42" name="Term Source REF ()         " totalsRowFunction="none"/>
-    <tableColumn id="43" name="Term Accession Number ()         " totalsRowFunction="none"/>
-    <tableColumn id="44" name="Characteristic [sample prep protocol]" totalsRowFunction="none"/>
-    <tableColumn id="45" name="Term Source REF ()          " totalsRowFunction="none"/>
-    <tableColumn id="46" name="Term Accession Number ()          " totalsRowFunction="none"/>
-    <tableColumn id="47" name="Characteristic [resuspension volume]" totalsRowFunction="none"/>
-    <tableColumn id="48" name="Term Source REF ()           " totalsRowFunction="none"/>
-    <tableColumn id="49" name="Term Accession Number ()           " totalsRowFunction="none"/>
-    <tableColumn id="50" name="Output [Sample Name]" totalsRowFunction="none"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Input [Source Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parameter [sample submission date]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF ()"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number ()"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Characteristic [organism]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Term Source REF (OBI:0100026)"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Accession Number (OBI:0100026)"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Characteristic [genotype]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Term Source REF (EFO:0000513)"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Term Accession Number (EFO:0000513)"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Characteristic [biological replicate]"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Term Source REF (DPBO:0000042)"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Term Accession Number (DPBO:0000042)"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Factor [condition]"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Term Source REF () "/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Term Accession Number () "/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Factor [condition.2]"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Term Source REF ()  "/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Term Accession Number ()  "/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Factor [condition.3]"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Term Source REF ()   "/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Term Accession Number ()   "/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Characteristic [Light Cycle]"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Term Source REF (NCIT:C90419)"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Term Accession Number (NCIT:C90419)"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Characteristic [Light intensity]"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Term Source REF ()    "/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Term Accession Number ()    "/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Characteristic [shaker rpm]"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Term Source REF ()     "/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Term Accession Number ()     "/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Characteristic [cultivation device]"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Term Source REF ()      "/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Term Accession Number ()      "/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Characteristic [cell number]"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Term Source REF ()       "/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Term Accession Number ()       "/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Characteristic [OD units]"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Term Source REF ()        "/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Term Accession Number ()        "/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Characteristic [sampling protocol]"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Term Source REF ()         "/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Term Accession Number ()         "/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Characteristic [sample prep protocol]"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Term Source REF ()          "/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Term Accession Number ()          "/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Characteristic [resuspension volume]"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Term Source REF ()           "/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Term Accession Number ()           "/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Output [Sample Name]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,16 +754,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -753,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -761,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -769,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -777,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -785,7 +808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -793,52 +816,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -846,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -854,52 +877,55 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -908,17 +934,23 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{9B4AC9A2-81A8-4782-9FB0-E6E61AF08587}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1070,7 +1102,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1224,7 +1256,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>